<commit_message>
fixed absolute paths. Fixed update bug. Updated dataset to include the grand final
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Geelong_stats.xlsx
+++ b/AFL_ML/Data/Geelong_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:KZ102"/>
+  <dimension ref="A1:LA102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="IO1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="JC11" activeCellId="0" sqref="JC11"/>
@@ -1389,8 +1389,11 @@
       <c r="KY1" s="2" t="n">
         <v>10748</v>
       </c>
-      <c r="KZ1" t="n">
+      <c r="KZ1" s="2" t="n">
         <v>10748</v>
+      </c>
+      <c r="LA1" t="n">
+        <v>10750</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="1">
@@ -2329,7 +2332,10 @@
       <c r="KY2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="KZ2" t="n">
+      <c r="KZ2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="LA2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -3269,8 +3275,11 @@
       <c r="KY3" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="KZ3" t="n">
+      <c r="KZ3" s="2" t="n">
         <v>27</v>
+      </c>
+      <c r="LA3" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="1">
@@ -4209,7 +4218,10 @@
       <c r="KY4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KZ4" t="n">
+      <c r="KZ4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LA4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5149,7 +5161,10 @@
       <c r="KY5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KZ5" t="n">
+      <c r="KZ5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LA5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6089,8 +6104,11 @@
       <c r="KY6" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="KZ6" t="n">
+      <c r="KZ6" s="2" t="n">
         <v>120</v>
+      </c>
+      <c r="LA6" t="n">
+        <v>133</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="1">
@@ -7029,8 +7047,11 @@
       <c r="KY7" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="KZ7" t="n">
+      <c r="KZ7" s="2" t="n">
         <v>49</v>
+      </c>
+      <c r="LA7" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="1">
@@ -7969,8 +7990,11 @@
       <c r="KY8" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="KZ8" t="n">
+      <c r="KZ8" s="2" t="n">
         <v>71</v>
+      </c>
+      <c r="LA8" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="1">
@@ -8909,7 +8933,10 @@
       <c r="KY9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KZ9" t="n">
+      <c r="KZ9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LA9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9849,8 +9876,11 @@
       <c r="KY10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KZ10" t="n">
+      <c r="KZ10" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="LA10" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="1">
@@ -10789,8 +10819,11 @@
       <c r="KY11" s="2" t="n">
         <v>209</v>
       </c>
-      <c r="KZ11" t="n">
+      <c r="KZ11" s="2" t="n">
         <v>209</v>
+      </c>
+      <c r="LA11" t="n">
+        <v>253</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="1">
@@ -11729,8 +11762,11 @@
       <c r="KY12" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="KZ12" t="n">
+      <c r="KZ12" s="2" t="n">
         <v>152</v>
+      </c>
+      <c r="LA12" t="n">
+        <v>142</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="1">
@@ -12669,8 +12705,11 @@
       <c r="KY13" s="2" t="n">
         <v>361</v>
       </c>
-      <c r="KZ13" t="n">
+      <c r="KZ13" s="2" t="n">
         <v>361</v>
+      </c>
+      <c r="LA13" t="n">
+        <v>395</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="1">
@@ -13609,8 +13648,11 @@
       <c r="KY14" s="2" t="n">
         <v>1.38</v>
       </c>
-      <c r="KZ14" t="n">
+      <c r="KZ14" s="2" t="n">
         <v>1.38</v>
+      </c>
+      <c r="LA14" t="n">
+        <v>1.78</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="1">
@@ -14549,8 +14591,11 @@
       <c r="KY15" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="KZ15" t="n">
+      <c r="KZ15" s="2" t="n">
         <v>102</v>
+      </c>
+      <c r="LA15" t="n">
+        <v>124</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="1">
@@ -15489,8 +15534,11 @@
       <c r="KY16" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="KZ16" t="n">
+      <c r="KZ16" s="2" t="n">
         <v>65</v>
+      </c>
+      <c r="LA16" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="1">
@@ -16429,8 +16477,11 @@
       <c r="KY17" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KZ17" t="n">
+      <c r="KZ17" s="2" t="n">
         <v>41</v>
+      </c>
+      <c r="LA17" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="1">
@@ -17369,8 +17420,11 @@
       <c r="KY18" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KZ18" t="n">
+      <c r="KZ18" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="LA18" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="1">
@@ -18309,8 +18363,11 @@
       <c r="KY19" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="KZ19" t="n">
+      <c r="KZ19" s="2" t="n">
         <v>22</v>
+      </c>
+      <c r="LA19" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="1">
@@ -19249,8 +19306,11 @@
       <c r="KY20" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="KZ20" t="n">
+      <c r="KZ20" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="LA20" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="1">
@@ -20189,7 +20249,10 @@
       <c r="KY21" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KZ21" t="n">
+      <c r="KZ21" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LA21" t="n">
         <v>14</v>
       </c>
     </row>
@@ -21129,8 +21192,11 @@
       <c r="KY22" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="KZ22" t="n">
+      <c r="KZ22" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="LA22" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="1">
@@ -22069,7 +22135,10 @@
       <c r="KY23" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KZ23" t="n">
+      <c r="KZ23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LA23" t="n">
         <v>2</v>
       </c>
     </row>
@@ -23009,8 +23078,11 @@
       <c r="KY24" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="KZ24" t="n">
+      <c r="KZ24" s="2" t="n">
         <v>30</v>
+      </c>
+      <c r="LA24" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="1">
@@ -23949,8 +24021,11 @@
       <c r="KY25" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="KZ25" t="n">
+      <c r="KZ25" s="2" t="n">
         <v>60</v>
+      </c>
+      <c r="LA25" t="n">
+        <v>60.6</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="1">
@@ -24889,8 +24964,11 @@
       <c r="KY26" s="2" t="n">
         <v>20.06</v>
       </c>
-      <c r="KZ26" t="n">
+      <c r="KZ26" s="2" t="n">
         <v>20.06</v>
+      </c>
+      <c r="LA26" t="n">
+        <v>19.75</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="1">
@@ -25829,8 +25907,11 @@
       <c r="KY27" s="2" t="n">
         <v>12.03</v>
       </c>
-      <c r="KZ27" t="n">
+      <c r="KZ27" s="2" t="n">
         <v>12.03</v>
+      </c>
+      <c r="LA27" t="n">
+        <v>11.97</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="1">
@@ -26769,8 +26850,11 @@
       <c r="KY28" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KZ28" t="n">
+      <c r="KZ28" s="2" t="n">
         <v>37</v>
+      </c>
+      <c r="LA28" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="1">
@@ -27709,8 +27793,11 @@
       <c r="KY29" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="KZ29" t="n">
+      <c r="KZ29" s="2" t="n">
         <v>55</v>
+      </c>
+      <c r="LA29" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="1">
@@ -28649,8 +28736,11 @@
       <c r="KY30" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="KZ30" t="n">
+      <c r="KZ30" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="LA30" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="1">
@@ -29589,8 +29679,11 @@
       <c r="KY31" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="KZ31" t="n">
+      <c r="KZ31" s="2" t="n">
         <v>59</v>
+      </c>
+      <c r="LA31" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="1">
@@ -30529,8 +30622,11 @@
       <c r="KY32" s="2" t="n">
         <v>1.97</v>
       </c>
-      <c r="KZ32" t="n">
+      <c r="KZ32" s="2" t="n">
         <v>1.97</v>
+      </c>
+      <c r="LA32" t="n">
+        <v>1.91</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="1">
@@ -31469,8 +31565,11 @@
       <c r="KY33" s="2" t="n">
         <v>3.28</v>
       </c>
-      <c r="KZ33" t="n">
+      <c r="KZ33" s="2" t="n">
         <v>3.28</v>
+      </c>
+      <c r="LA33" t="n">
+        <v>3.15</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="1">
@@ -32409,8 +32508,11 @@
       <c r="KY34" s="2" t="n">
         <v>47.5</v>
       </c>
-      <c r="KZ34" t="n">
+      <c r="KZ34" s="2" t="n">
         <v>47.5</v>
+      </c>
+      <c r="LA34" t="n">
+        <v>49.2</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="1">
@@ -33349,8 +33451,11 @@
       <c r="KY35" s="2" t="n">
         <v>30.5</v>
       </c>
-      <c r="KZ35" t="n">
+      <c r="KZ35" s="2" t="n">
         <v>30.5</v>
+      </c>
+      <c r="LA35" t="n">
+        <v>31.7</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="1">
@@ -34289,8 +34394,11 @@
       <c r="KY36" s="2" t="n">
         <v>188.9</v>
       </c>
-      <c r="KZ36" t="n">
+      <c r="KZ36" s="2" t="n">
         <v>188.9</v>
+      </c>
+      <c r="LA36" t="n">
+        <v>188.5</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="1">
@@ -35229,8 +35337,11 @@
       <c r="KY37" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="KZ37" t="n">
+      <c r="KZ37" s="2" t="n">
         <v>88</v>
+      </c>
+      <c r="LA37" t="n">
+        <v>88.2</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="1">
@@ -36169,8 +36280,11 @@
       <c r="KY38" s="2" t="n">
         <v>28.33</v>
       </c>
-      <c r="KZ38" t="n">
+      <c r="KZ38" s="2" t="n">
         <v>28.33</v>
+      </c>
+      <c r="LA38" t="n">
+        <v>28.58</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="1">
@@ -37109,8 +37223,11 @@
       <c r="KY39" s="2" t="n">
         <v>163.1</v>
       </c>
-      <c r="KZ39" t="n">
+      <c r="KZ39" s="2" t="n">
         <v>163.1</v>
+      </c>
+      <c r="LA39" t="n">
+        <v>167.6</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="1">
@@ -38049,8 +38166,11 @@
       <c r="KY40" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="KZ40" t="n">
+      <c r="KZ40" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="LA40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="1">
@@ -38989,7 +39109,10 @@
       <c r="KY41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="KZ41" t="n">
+      <c r="KZ41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LA41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -39929,8 +40052,11 @@
       <c r="KY42" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KZ42" t="n">
+      <c r="KZ42" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="LA42" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="1">
@@ -40869,7 +40995,10 @@
       <c r="KY43" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KZ43" t="n">
+      <c r="KZ43" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="LA43" t="n">
         <v>13</v>
       </c>
     </row>
@@ -41809,8 +41938,11 @@
       <c r="KY44" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="KZ44" t="n">
+      <c r="KZ44" s="2" t="n">
         <v>125</v>
+      </c>
+      <c r="LA44" t="n">
+        <v>151</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="1">
@@ -42749,8 +42881,11 @@
       <c r="KY45" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="KZ45" t="n">
+      <c r="KZ45" s="2" t="n">
         <v>230</v>
+      </c>
+      <c r="LA45" t="n">
+        <v>253</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="1">
@@ -43689,8 +43824,11 @@
       <c r="KY46" s="2" t="n">
         <v>274</v>
       </c>
-      <c r="KZ46" t="n">
+      <c r="KZ46" s="2" t="n">
         <v>274</v>
+      </c>
+      <c r="LA46" t="n">
+        <v>296</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="1">
@@ -44629,8 +44767,11 @@
       <c r="KY47" s="2" t="n">
         <v>75.90000000000001</v>
       </c>
-      <c r="KZ47" t="n">
+      <c r="KZ47" s="2" t="n">
         <v>75.90000000000001</v>
+      </c>
+      <c r="LA47" t="n">
+        <v>74.90000000000001</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="1">
@@ -45569,8 +45710,11 @@
       <c r="KY48" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="KZ48" t="n">
+      <c r="KZ48" s="2" t="n">
         <v>55</v>
+      </c>
+      <c r="LA48" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="1">
@@ -46509,8 +46653,11 @@
       <c r="KY49" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="KZ49" t="n">
+      <c r="KZ49" s="2" t="n">
         <v>15</v>
+      </c>
+      <c r="LA49" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="1">
@@ -47449,8 +47596,11 @@
       <c r="KY50" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="KZ50" t="n">
+      <c r="KZ50" s="2" t="n">
         <v>15</v>
+      </c>
+      <c r="LA50" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="1">
@@ -48389,8 +48539,11 @@
       <c r="KY51" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KZ51" t="n">
+      <c r="KZ51" s="2" t="n">
         <v>37</v>
+      </c>
+      <c r="LA51" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="1">
@@ -49329,8 +49482,11 @@
       <c r="KY52" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="KZ52" t="n">
+      <c r="KZ52" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="LA52" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="1">
@@ -50269,8 +50425,11 @@
       <c r="KY53" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="KZ53" t="n">
+      <c r="KZ53" s="2" t="n">
         <v>48</v>
+      </c>
+      <c r="LA53" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="1">
@@ -51209,8 +51368,11 @@
       <c r="KY54" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KZ54" t="n">
+      <c r="KZ54" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="LA54" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="1">
@@ -52149,7 +52311,10 @@
       <c r="KY55" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KZ55" t="n">
+      <c r="KZ55" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LA55" t="n">
         <v>14</v>
       </c>
     </row>
@@ -53089,8 +53254,11 @@
       <c r="KY56" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="KZ56" t="n">
+      <c r="KZ56" s="2" t="n">
         <v>77.8</v>
+      </c>
+      <c r="LA56" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="1">
@@ -54029,8 +54197,11 @@
       <c r="KY57" s="2" t="n">
         <v>197</v>
       </c>
-      <c r="KZ57" t="n">
+      <c r="KZ57" s="2" t="n">
         <v>197</v>
+      </c>
+      <c r="LA57" t="n">
+        <v>166</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="1">
@@ -54969,8 +55140,11 @@
       <c r="KY58" s="2" t="n">
         <v>99</v>
       </c>
-      <c r="KZ58" t="n">
+      <c r="KZ58" s="2" t="n">
         <v>99</v>
+      </c>
+      <c r="LA58" t="n">
+        <v>138</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="1">
@@ -55909,8 +56083,11 @@
       <c r="KY59" s="2" t="n">
         <v>296</v>
       </c>
-      <c r="KZ59" t="n">
+      <c r="KZ59" s="2" t="n">
         <v>296</v>
+      </c>
+      <c r="LA59" t="n">
+        <v>304</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="1">
@@ -56849,8 +57026,11 @@
       <c r="KY60" s="2" t="n">
         <v>1.99</v>
       </c>
-      <c r="KZ60" t="n">
+      <c r="KZ60" s="2" t="n">
         <v>1.99</v>
+      </c>
+      <c r="LA60" t="n">
+        <v>1.2</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="1">
@@ -57789,8 +57969,11 @@
       <c r="KY61" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="KZ61" t="n">
+      <c r="KZ61" s="2" t="n">
         <v>88</v>
+      </c>
+      <c r="LA61" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="1">
@@ -58729,8 +58912,11 @@
       <c r="KY62" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="KZ62" t="n">
+      <c r="KZ62" s="2" t="n">
         <v>68</v>
+      </c>
+      <c r="LA62" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="1">
@@ -59669,8 +59855,11 @@
       <c r="KY63" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KZ63" t="n">
+      <c r="KZ63" s="2" t="n">
         <v>41</v>
+      </c>
+      <c r="LA63" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="1">
@@ -60609,8 +60798,11 @@
       <c r="KY64" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="KZ64" t="n">
+      <c r="KZ64" s="2" t="n">
         <v>22</v>
+      </c>
+      <c r="LA64" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="1">
@@ -61549,8 +61741,11 @@
       <c r="KY65" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KZ65" t="n">
+      <c r="KZ65" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="LA65" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="1">
@@ -62489,8 +62684,11 @@
       <c r="KY66" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KZ66" t="n">
+      <c r="KZ66" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LA66" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="1">
@@ -63429,8 +63627,11 @@
       <c r="KY67" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KZ67" t="n">
+      <c r="KZ67" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LA67" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="1">
@@ -64369,8 +64570,11 @@
       <c r="KY68" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KZ68" t="n">
+      <c r="KZ68" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LA68" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="1">
@@ -65309,8 +65513,11 @@
       <c r="KY69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KZ69" t="n">
+      <c r="KZ69" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="LA69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="1">
@@ -66249,8 +66456,11 @@
       <c r="KY70" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KZ70" t="n">
+      <c r="KZ70" s="2" t="n">
         <v>14</v>
+      </c>
+      <c r="LA70" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="1">
@@ -67189,8 +67399,11 @@
       <c r="KY71" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KZ71" t="n">
+      <c r="KZ71" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="LA71" t="n">
+        <v>66.7</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="1">
@@ -68129,8 +68342,11 @@
       <c r="KY72" s="2" t="n">
         <v>42.29</v>
       </c>
-      <c r="KZ72" t="n">
+      <c r="KZ72" s="2" t="n">
         <v>42.29</v>
+      </c>
+      <c r="LA72" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="1">
@@ -69069,8 +69285,11 @@
       <c r="KY73" s="2" t="n">
         <v>21.14</v>
       </c>
-      <c r="KZ73" t="n">
+      <c r="KZ73" s="2" t="n">
         <v>21.14</v>
+      </c>
+      <c r="LA73" t="n">
+        <v>25.33</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="1">
@@ -70009,8 +70228,11 @@
       <c r="KY74" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="KZ74" t="n">
+      <c r="KZ74" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="LA74" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="1">
@@ -70949,8 +71171,11 @@
       <c r="KY75" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KZ75" t="n">
+      <c r="KZ75" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="LA75" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="1">
@@ -71889,8 +72114,11 @@
       <c r="KY76" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KZ76" t="n">
+      <c r="KZ76" s="2" t="n">
         <v>41</v>
+      </c>
+      <c r="LA76" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="1">
@@ -72829,8 +73057,11 @@
       <c r="KY77" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="KZ77" t="n">
+      <c r="KZ77" s="2" t="n">
         <v>46</v>
+      </c>
+      <c r="LA77" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="1">
@@ -73769,8 +74000,11 @@
       <c r="KY78" s="2" t="n">
         <v>3.29</v>
       </c>
-      <c r="KZ78" t="n">
+      <c r="KZ78" s="2" t="n">
         <v>3.29</v>
+      </c>
+      <c r="LA78" t="n">
+        <v>2.67</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="1">
@@ -74709,8 +74943,11 @@
       <c r="KY79" s="2" t="n">
         <v>6.57</v>
       </c>
-      <c r="KZ79" t="n">
+      <c r="KZ79" s="2" t="n">
         <v>6.57</v>
+      </c>
+      <c r="LA79" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="1">
@@ -75649,8 +75886,11 @@
       <c r="KY80" s="2" t="n">
         <v>30.4</v>
       </c>
-      <c r="KZ80" t="n">
+      <c r="KZ80" s="2" t="n">
         <v>30.4</v>
+      </c>
+      <c r="LA80" t="n">
+        <v>34.4</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="1">
@@ -76589,8 +76829,11 @@
       <c r="KY81" s="2" t="n">
         <v>15.2</v>
       </c>
-      <c r="KZ81" t="n">
+      <c r="KZ81" s="2" t="n">
         <v>15.2</v>
+      </c>
+      <c r="LA81" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="1">
@@ -77529,8 +77772,11 @@
       <c r="KY82" s="2" t="n">
         <v>187.9</v>
       </c>
-      <c r="KZ82" t="n">
+      <c r="KZ82" s="2" t="n">
         <v>187.9</v>
+      </c>
+      <c r="LA82" t="n">
+        <v>187.6</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="1">
@@ -78469,8 +78715,11 @@
       <c r="KY83" s="2" t="n">
         <v>87.8</v>
       </c>
-      <c r="KZ83" t="n">
+      <c r="KZ83" s="2" t="n">
         <v>87.8</v>
+      </c>
+      <c r="LA83" t="n">
+        <v>86.3</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="1">
@@ -79409,8 +79658,11 @@
       <c r="KY84" s="2" t="n">
         <v>25.66</v>
       </c>
-      <c r="KZ84" t="n">
+      <c r="KZ84" s="2" t="n">
         <v>25.66</v>
+      </c>
+      <c r="LA84" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="1">
@@ -80349,8 +80601,11 @@
       <c r="KY85" s="2" t="n">
         <v>116.6</v>
       </c>
-      <c r="KZ85" t="n">
+      <c r="KZ85" s="2" t="n">
         <v>116.6</v>
+      </c>
+      <c r="LA85" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="1">
@@ -81289,8 +81544,11 @@
       <c r="KY86" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="KZ86" t="n">
+      <c r="KZ86" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="LA86" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="1">
@@ -82229,8 +82487,11 @@
       <c r="KY87" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="KZ87" t="n">
+      <c r="KZ87" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LA87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="1">
@@ -83169,8 +83430,11 @@
       <c r="KY88" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="KZ88" t="n">
+      <c r="KZ88" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="LA88" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="1">
@@ -84109,8 +84373,11 @@
       <c r="KY89" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KZ89" t="n">
+      <c r="KZ89" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="LA89" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="1">
@@ -85049,8 +85316,11 @@
       <c r="KY90" s="2" t="n">
         <v>117</v>
       </c>
-      <c r="KZ90" t="n">
+      <c r="KZ90" s="2" t="n">
         <v>117</v>
+      </c>
+      <c r="LA90" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="1">
@@ -85989,8 +86259,11 @@
       <c r="KY91" s="2" t="n">
         <v>177</v>
       </c>
-      <c r="KZ91" t="n">
+      <c r="KZ91" s="2" t="n">
         <v>177</v>
+      </c>
+      <c r="LA91" t="n">
+        <v>189</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="1">
@@ -86929,8 +87202,11 @@
       <c r="KY92" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="KZ92" t="n">
+      <c r="KZ92" s="2" t="n">
         <v>200</v>
+      </c>
+      <c r="LA92" t="n">
+        <v>232</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="1">
@@ -87869,8 +88145,11 @@
       <c r="KY93" s="2" t="n">
         <v>67.59999999999999</v>
       </c>
-      <c r="KZ93" t="n">
+      <c r="KZ93" s="2" t="n">
         <v>67.59999999999999</v>
+      </c>
+      <c r="LA93" t="n">
+        <v>76.3</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="1">
@@ -88809,8 +89088,11 @@
       <c r="KY94" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KZ94" t="n">
+      <c r="KZ94" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="LA94" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="1">
@@ -89749,8 +90031,11 @@
       <c r="KY95" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KZ95" t="n">
+      <c r="KZ95" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="LA95" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="1">
@@ -90689,8 +90974,11 @@
       <c r="KY96" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="KZ96" t="n">
+      <c r="KZ96" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="LA96" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="1">
@@ -91629,8 +91917,11 @@
       <c r="KY97" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="KZ97" t="n">
+      <c r="KZ97" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="LA97" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="1">
@@ -92569,8 +92860,11 @@
       <c r="KY98" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KZ98" t="n">
+      <c r="KZ98" s="2" t="n">
         <v>41</v>
+      </c>
+      <c r="LA98" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="1">
@@ -93509,8 +93803,11 @@
       <c r="KY99" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KZ99" t="n">
+      <c r="KZ99" s="2" t="n">
         <v>37</v>
+      </c>
+      <c r="LA99" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="1">
@@ -94449,8 +94746,11 @@
       <c r="KY100" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KZ100" t="n">
+      <c r="KZ100" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="LA100" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="1">
@@ -95389,8 +95689,11 @@
       <c r="KY101" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KZ101" t="n">
+      <c r="KZ101" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LA101" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="1">
@@ -96329,8 +96632,11 @@
       <c r="KY102" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="KZ102" t="n">
+      <c r="KZ102" s="2" t="n">
         <v>100</v>
+      </c>
+      <c r="LA102" t="n">
+        <v>62.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed year to 2023. Added functionality for extra round. retrained model to use all 2022 data. added alias method for stadium name
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Geelong_stats.xlsx
+++ b/AFL_ML/Data/Geelong_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:LA102"/>
+  <dimension ref="A1:LC102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="IO1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="JC11" activeCellId="0" sqref="JC11"/>
@@ -1392,7 +1392,13 @@
       <c r="KZ1" s="2" t="n">
         <v>10748</v>
       </c>
-      <c r="LA1" t="n">
+      <c r="LA1" s="2" t="n">
+        <v>10750</v>
+      </c>
+      <c r="LB1" s="2" t="n">
+        <v>10750</v>
+      </c>
+      <c r="LC1" t="n">
         <v>10750</v>
       </c>
     </row>
@@ -2335,7 +2341,13 @@
       <c r="KZ2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="LA2" t="n">
+      <c r="LA2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="LB2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="LC2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -3278,7 +3290,13 @@
       <c r="KZ3" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="LA3" t="n">
+      <c r="LA3" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="LB3" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="LC3" t="n">
         <v>28</v>
       </c>
     </row>
@@ -4221,7 +4239,13 @@
       <c r="KZ4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="LA4" t="n">
+      <c r="LA4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LC4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5164,7 +5188,13 @@
       <c r="KZ5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="LA5" t="n">
+      <c r="LA5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LC5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6107,7 +6137,13 @@
       <c r="KZ6" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="LA6" t="n">
+      <c r="LA6" s="2" t="n">
+        <v>133</v>
+      </c>
+      <c r="LB6" s="2" t="n">
+        <v>133</v>
+      </c>
+      <c r="LC6" t="n">
         <v>133</v>
       </c>
     </row>
@@ -7050,7 +7086,13 @@
       <c r="KZ7" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="LA7" t="n">
+      <c r="LA7" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="LB7" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="LC7" t="n">
         <v>52</v>
       </c>
     </row>
@@ -7993,7 +8035,13 @@
       <c r="KZ8" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="LA8" t="n">
+      <c r="LA8" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="LB8" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="LC8" t="n">
         <v>81</v>
       </c>
     </row>
@@ -8936,7 +8984,13 @@
       <c r="KZ9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="LA9" t="n">
+      <c r="LA9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LB9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LC9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9879,7 +9933,13 @@
       <c r="KZ10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="LA10" t="n">
+      <c r="LA10" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="LB10" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="LC10" t="n">
         <v>16</v>
       </c>
     </row>
@@ -10822,7 +10882,13 @@
       <c r="KZ11" s="2" t="n">
         <v>209</v>
       </c>
-      <c r="LA11" t="n">
+      <c r="LA11" s="2" t="n">
+        <v>253</v>
+      </c>
+      <c r="LB11" s="2" t="n">
+        <v>253</v>
+      </c>
+      <c r="LC11" t="n">
         <v>253</v>
       </c>
     </row>
@@ -11765,7 +11831,13 @@
       <c r="KZ12" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="LA12" t="n">
+      <c r="LA12" s="2" t="n">
+        <v>142</v>
+      </c>
+      <c r="LB12" s="2" t="n">
+        <v>142</v>
+      </c>
+      <c r="LC12" t="n">
         <v>142</v>
       </c>
     </row>
@@ -12708,7 +12780,13 @@
       <c r="KZ13" s="2" t="n">
         <v>361</v>
       </c>
-      <c r="LA13" t="n">
+      <c r="LA13" s="2" t="n">
+        <v>395</v>
+      </c>
+      <c r="LB13" s="2" t="n">
+        <v>395</v>
+      </c>
+      <c r="LC13" t="n">
         <v>395</v>
       </c>
     </row>
@@ -13651,7 +13729,13 @@
       <c r="KZ14" s="2" t="n">
         <v>1.38</v>
       </c>
-      <c r="LA14" t="n">
+      <c r="LA14" s="2" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="LB14" s="2" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="LC14" t="n">
         <v>1.78</v>
       </c>
     </row>
@@ -14594,7 +14678,13 @@
       <c r="KZ15" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="LA15" t="n">
+      <c r="LA15" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="LB15" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="LC15" t="n">
         <v>124</v>
       </c>
     </row>
@@ -15537,7 +15627,13 @@
       <c r="KZ16" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="LA16" t="n">
+      <c r="LA16" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="LB16" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="LC16" t="n">
         <v>56</v>
       </c>
     </row>
@@ -16480,7 +16576,13 @@
       <c r="KZ17" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="LA17" t="n">
+      <c r="LA17" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="LB17" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="LC17" t="n">
         <v>44</v>
       </c>
     </row>
@@ -17423,7 +17525,13 @@
       <c r="KZ18" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="LA18" t="n">
+      <c r="LA18" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LB18" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LC18" t="n">
         <v>17</v>
       </c>
     </row>
@@ -18366,7 +18474,13 @@
       <c r="KZ19" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="LA19" t="n">
+      <c r="LA19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LB19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LC19" t="n">
         <v>18</v>
       </c>
     </row>
@@ -19309,7 +19423,13 @@
       <c r="KZ20" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="LA20" t="n">
+      <c r="LA20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="LB20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="LC20" t="n">
         <v>20</v>
       </c>
     </row>
@@ -20252,7 +20372,13 @@
       <c r="KZ21" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="LA21" t="n">
+      <c r="LA21" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LB21" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LC21" t="n">
         <v>14</v>
       </c>
     </row>
@@ -21195,7 +21321,13 @@
       <c r="KZ22" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="LA22" t="n">
+      <c r="LA22" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LB22" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LC22" t="n">
         <v>11</v>
       </c>
     </row>
@@ -22138,7 +22270,13 @@
       <c r="KZ23" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="LA23" t="n">
+      <c r="LA23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LB23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LC23" t="n">
         <v>2</v>
       </c>
     </row>
@@ -23081,7 +23219,13 @@
       <c r="KZ24" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="LA24" t="n">
+      <c r="LA24" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LB24" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LC24" t="n">
         <v>33</v>
       </c>
     </row>
@@ -24024,7 +24168,13 @@
       <c r="KZ25" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="LA25" t="n">
+      <c r="LA25" s="2" t="n">
+        <v>60.6</v>
+      </c>
+      <c r="LB25" s="2" t="n">
+        <v>60.6</v>
+      </c>
+      <c r="LC25" t="n">
         <v>60.6</v>
       </c>
     </row>
@@ -24967,7 +25117,13 @@
       <c r="KZ26" s="2" t="n">
         <v>20.06</v>
       </c>
-      <c r="LA26" t="n">
+      <c r="LA26" s="2" t="n">
+        <v>19.75</v>
+      </c>
+      <c r="LB26" s="2" t="n">
+        <v>19.75</v>
+      </c>
+      <c r="LC26" t="n">
         <v>19.75</v>
       </c>
     </row>
@@ -25910,7 +26066,13 @@
       <c r="KZ27" s="2" t="n">
         <v>12.03</v>
       </c>
-      <c r="LA27" t="n">
+      <c r="LA27" s="2" t="n">
+        <v>11.97</v>
+      </c>
+      <c r="LB27" s="2" t="n">
+        <v>11.97</v>
+      </c>
+      <c r="LC27" t="n">
         <v>11.97</v>
       </c>
     </row>
@@ -26853,7 +27015,13 @@
       <c r="KZ28" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="LA28" t="n">
+      <c r="LA28" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LB28" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LC28" t="n">
         <v>33</v>
       </c>
     </row>
@@ -27796,7 +27964,13 @@
       <c r="KZ29" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="LA29" t="n">
+      <c r="LA29" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LB29" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LC29" t="n">
         <v>54</v>
       </c>
     </row>
@@ -28739,7 +28913,13 @@
       <c r="KZ30" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="LA30" t="n">
+      <c r="LA30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="LB30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="LC30" t="n">
         <v>23</v>
       </c>
     </row>
@@ -29682,7 +29862,13 @@
       <c r="KZ31" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="LA31" t="n">
+      <c r="LA31" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="LB31" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="LC31" t="n">
         <v>63</v>
       </c>
     </row>
@@ -30625,7 +30811,13 @@
       <c r="KZ32" s="2" t="n">
         <v>1.97</v>
       </c>
-      <c r="LA32" t="n">
+      <c r="LA32" s="2" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="LB32" s="2" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="LC32" t="n">
         <v>1.91</v>
       </c>
     </row>
@@ -31568,7 +31760,13 @@
       <c r="KZ33" s="2" t="n">
         <v>3.28</v>
       </c>
-      <c r="LA33" t="n">
+      <c r="LA33" s="2" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="LB33" s="2" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="LC33" t="n">
         <v>3.15</v>
       </c>
     </row>
@@ -32511,7 +32709,13 @@
       <c r="KZ34" s="2" t="n">
         <v>47.5</v>
       </c>
-      <c r="LA34" t="n">
+      <c r="LA34" s="2" t="n">
+        <v>49.2</v>
+      </c>
+      <c r="LB34" s="2" t="n">
+        <v>49.2</v>
+      </c>
+      <c r="LC34" t="n">
         <v>49.2</v>
       </c>
     </row>
@@ -33454,7 +33658,13 @@
       <c r="KZ35" s="2" t="n">
         <v>30.5</v>
       </c>
-      <c r="LA35" t="n">
+      <c r="LA35" s="2" t="n">
+        <v>31.7</v>
+      </c>
+      <c r="LB35" s="2" t="n">
+        <v>31.7</v>
+      </c>
+      <c r="LC35" t="n">
         <v>31.7</v>
       </c>
     </row>
@@ -34397,7 +34607,13 @@
       <c r="KZ36" s="2" t="n">
         <v>188.9</v>
       </c>
-      <c r="LA36" t="n">
+      <c r="LA36" s="2" t="n">
+        <v>188.5</v>
+      </c>
+      <c r="LB36" s="2" t="n">
+        <v>188.5</v>
+      </c>
+      <c r="LC36" t="n">
         <v>188.5</v>
       </c>
     </row>
@@ -35340,7 +35556,13 @@
       <c r="KZ37" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="LA37" t="n">
+      <c r="LA37" s="2" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="LB37" s="2" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="LC37" t="n">
         <v>88.2</v>
       </c>
     </row>
@@ -36283,7 +36505,13 @@
       <c r="KZ38" s="2" t="n">
         <v>28.33</v>
       </c>
-      <c r="LA38" t="n">
+      <c r="LA38" s="2" t="n">
+        <v>28.58</v>
+      </c>
+      <c r="LB38" s="2" t="n">
+        <v>28.58</v>
+      </c>
+      <c r="LC38" t="n">
         <v>28.58</v>
       </c>
     </row>
@@ -37226,7 +37454,13 @@
       <c r="KZ39" s="2" t="n">
         <v>163.1</v>
       </c>
-      <c r="LA39" t="n">
+      <c r="LA39" s="2" t="n">
+        <v>167.6</v>
+      </c>
+      <c r="LB39" s="2" t="n">
+        <v>167.6</v>
+      </c>
+      <c r="LC39" t="n">
         <v>167.6</v>
       </c>
     </row>
@@ -38169,7 +38403,13 @@
       <c r="KZ40" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="LA40" t="n">
+      <c r="LA40" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LB40" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LC40" t="n">
         <v>2</v>
       </c>
     </row>
@@ -39112,7 +39352,13 @@
       <c r="KZ41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="LA41" t="n">
+      <c r="LA41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LB41" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LC41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -40055,7 +40301,13 @@
       <c r="KZ42" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="LA42" t="n">
+      <c r="LA42" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LB42" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LC42" t="n">
         <v>3</v>
       </c>
     </row>
@@ -40998,7 +41250,13 @@
       <c r="KZ43" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="LA43" t="n">
+      <c r="LA43" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="LB43" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="LC43" t="n">
         <v>13</v>
       </c>
     </row>
@@ -41941,7 +42199,13 @@
       <c r="KZ44" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="LA44" t="n">
+      <c r="LA44" s="2" t="n">
+        <v>151</v>
+      </c>
+      <c r="LB44" s="2" t="n">
+        <v>151</v>
+      </c>
+      <c r="LC44" t="n">
         <v>151</v>
       </c>
     </row>
@@ -42884,7 +43148,13 @@
       <c r="KZ45" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="LA45" t="n">
+      <c r="LA45" s="2" t="n">
+        <v>253</v>
+      </c>
+      <c r="LB45" s="2" t="n">
+        <v>253</v>
+      </c>
+      <c r="LC45" t="n">
         <v>253</v>
       </c>
     </row>
@@ -43827,7 +44097,13 @@
       <c r="KZ46" s="2" t="n">
         <v>274</v>
       </c>
-      <c r="LA46" t="n">
+      <c r="LA46" s="2" t="n">
+        <v>296</v>
+      </c>
+      <c r="LB46" s="2" t="n">
+        <v>296</v>
+      </c>
+      <c r="LC46" t="n">
         <v>296</v>
       </c>
     </row>
@@ -44770,7 +45046,13 @@
       <c r="KZ47" s="2" t="n">
         <v>75.90000000000001</v>
       </c>
-      <c r="LA47" t="n">
+      <c r="LA47" s="2" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="LB47" s="2" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="LC47" t="n">
         <v>74.90000000000001</v>
       </c>
     </row>
@@ -45713,7 +45995,13 @@
       <c r="KZ48" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="LA48" t="n">
+      <c r="LA48" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LB48" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LC48" t="n">
         <v>54</v>
       </c>
     </row>
@@ -46656,7 +46944,13 @@
       <c r="KZ49" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="LA49" t="n">
+      <c r="LA49" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LB49" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LC49" t="n">
         <v>6</v>
       </c>
     </row>
@@ -47599,7 +47893,13 @@
       <c r="KZ50" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="LA50" t="n">
+      <c r="LA50" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LB50" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LC50" t="n">
         <v>17</v>
       </c>
     </row>
@@ -48542,7 +48842,13 @@
       <c r="KZ51" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="LA51" t="n">
+      <c r="LA51" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LB51" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LC51" t="n">
         <v>33</v>
       </c>
     </row>
@@ -49485,7 +49791,13 @@
       <c r="KZ52" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="LA52" t="n">
+      <c r="LA52" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="LB52" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="LC52" t="n">
         <v>23</v>
       </c>
     </row>
@@ -50428,7 +50740,13 @@
       <c r="KZ53" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="LA53" t="n">
+      <c r="LA53" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="LB53" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="LC53" t="n">
         <v>43</v>
       </c>
     </row>
@@ -51371,7 +51689,13 @@
       <c r="KZ54" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="LA54" t="n">
+      <c r="LA54" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LB54" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LC54" t="n">
         <v>5</v>
       </c>
     </row>
@@ -52314,7 +52638,13 @@
       <c r="KZ55" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="LA55" t="n">
+      <c r="LA55" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LB55" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LC55" t="n">
         <v>14</v>
       </c>
     </row>
@@ -53257,7 +53587,13 @@
       <c r="KZ56" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="LA56" t="n">
+      <c r="LA56" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="LB56" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="LC56" t="n">
         <v>70</v>
       </c>
     </row>
@@ -54200,7 +54536,13 @@
       <c r="KZ57" s="2" t="n">
         <v>197</v>
       </c>
-      <c r="LA57" t="n">
+      <c r="LA57" s="2" t="n">
+        <v>166</v>
+      </c>
+      <c r="LB57" s="2" t="n">
+        <v>166</v>
+      </c>
+      <c r="LC57" t="n">
         <v>166</v>
       </c>
     </row>
@@ -55143,7 +55485,13 @@
       <c r="KZ58" s="2" t="n">
         <v>99</v>
       </c>
-      <c r="LA58" t="n">
+      <c r="LA58" s="2" t="n">
+        <v>138</v>
+      </c>
+      <c r="LB58" s="2" t="n">
+        <v>138</v>
+      </c>
+      <c r="LC58" t="n">
         <v>138</v>
       </c>
     </row>
@@ -56086,7 +56434,13 @@
       <c r="KZ59" s="2" t="n">
         <v>296</v>
       </c>
-      <c r="LA59" t="n">
+      <c r="LA59" s="2" t="n">
+        <v>304</v>
+      </c>
+      <c r="LB59" s="2" t="n">
+        <v>304</v>
+      </c>
+      <c r="LC59" t="n">
         <v>304</v>
       </c>
     </row>
@@ -57029,7 +57383,13 @@
       <c r="KZ60" s="2" t="n">
         <v>1.99</v>
       </c>
-      <c r="LA60" t="n">
+      <c r="LA60" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="LB60" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="LC60" t="n">
         <v>1.2</v>
       </c>
     </row>
@@ -57972,7 +58332,13 @@
       <c r="KZ61" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="LA61" t="n">
+      <c r="LA61" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="LB61" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="LC61" t="n">
         <v>62</v>
       </c>
     </row>
@@ -58915,7 +59281,13 @@
       <c r="KZ62" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="LA62" t="n">
+      <c r="LA62" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="LB62" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="LC62" t="n">
         <v>65</v>
       </c>
     </row>
@@ -59858,7 +60230,13 @@
       <c r="KZ63" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="LA63" t="n">
+      <c r="LA63" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="LB63" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="LC63" t="n">
         <v>24</v>
       </c>
     </row>
@@ -60801,7 +61179,13 @@
       <c r="KZ64" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="LA64" t="n">
+      <c r="LA64" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LB64" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LC64" t="n">
         <v>18</v>
       </c>
     </row>
@@ -61744,7 +62128,13 @@
       <c r="KZ65" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="LA65" t="n">
+      <c r="LA65" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LB65" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LC65" t="n">
         <v>17</v>
       </c>
     </row>
@@ -62687,7 +63077,13 @@
       <c r="KZ66" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LA66" t="n">
+      <c r="LA66" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LB66" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LC66" t="n">
         <v>8</v>
       </c>
     </row>
@@ -63630,7 +64026,13 @@
       <c r="KZ67" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LA67" t="n">
+      <c r="LA67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LB67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LC67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -64573,7 +64975,13 @@
       <c r="KZ68" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LA68" t="n">
+      <c r="LA68" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LB68" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LC68" t="n">
         <v>3</v>
       </c>
     </row>
@@ -65516,7 +65924,13 @@
       <c r="KZ69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="LA69" t="n">
+      <c r="LA69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LB69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LC69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -66459,7 +66873,13 @@
       <c r="KZ70" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="LA70" t="n">
+      <c r="LA70" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="LB70" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="LC70" t="n">
         <v>12</v>
       </c>
     </row>
@@ -67402,7 +67822,13 @@
       <c r="KZ71" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="LA71" t="n">
+      <c r="LA71" s="2" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="LB71" s="2" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="LC71" t="n">
         <v>66.7</v>
       </c>
     </row>
@@ -68345,7 +68771,13 @@
       <c r="KZ72" s="2" t="n">
         <v>42.29</v>
       </c>
-      <c r="LA72" t="n">
+      <c r="LA72" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="LB72" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="LC72" t="n">
         <v>38</v>
       </c>
     </row>
@@ -69288,7 +69720,13 @@
       <c r="KZ73" s="2" t="n">
         <v>21.14</v>
       </c>
-      <c r="LA73" t="n">
+      <c r="LA73" s="2" t="n">
+        <v>25.33</v>
+      </c>
+      <c r="LB73" s="2" t="n">
+        <v>25.33</v>
+      </c>
+      <c r="LC73" t="n">
         <v>25.33</v>
       </c>
     </row>
@@ -70231,7 +70669,13 @@
       <c r="KZ74" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="LA74" t="n">
+      <c r="LA74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="LB74" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="LC74" t="n">
         <v>37</v>
       </c>
     </row>
@@ -71174,7 +71618,13 @@
       <c r="KZ75" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="LA75" t="n">
+      <c r="LA75" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LB75" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LC75" t="n">
         <v>54</v>
       </c>
     </row>
@@ -72117,7 +72567,13 @@
       <c r="KZ76" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="LA76" t="n">
+      <c r="LA76" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LB76" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LC76" t="n">
         <v>45</v>
       </c>
     </row>
@@ -73060,7 +73516,13 @@
       <c r="KZ77" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="LA77" t="n">
+      <c r="LA77" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="LB77" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="LC77" t="n">
         <v>32</v>
       </c>
     </row>
@@ -74003,7 +74465,13 @@
       <c r="KZ78" s="2" t="n">
         <v>3.29</v>
       </c>
-      <c r="LA78" t="n">
+      <c r="LA78" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="LB78" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="LC78" t="n">
         <v>2.67</v>
       </c>
     </row>
@@ -74946,7 +75414,13 @@
       <c r="KZ79" s="2" t="n">
         <v>6.57</v>
       </c>
-      <c r="LA79" t="n">
+      <c r="LA79" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LB79" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LC79" t="n">
         <v>4</v>
       </c>
     </row>
@@ -75889,7 +76363,13 @@
       <c r="KZ80" s="2" t="n">
         <v>30.4</v>
       </c>
-      <c r="LA80" t="n">
+      <c r="LA80" s="2" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="LB80" s="2" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="LC80" t="n">
         <v>34.4</v>
       </c>
     </row>
@@ -76832,7 +77312,13 @@
       <c r="KZ81" s="2" t="n">
         <v>15.2</v>
       </c>
-      <c r="LA81" t="n">
+      <c r="LA81" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="LB81" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="LC81" t="n">
         <v>25</v>
       </c>
     </row>
@@ -77775,7 +78261,13 @@
       <c r="KZ82" s="2" t="n">
         <v>187.9</v>
       </c>
-      <c r="LA82" t="n">
+      <c r="LA82" s="2" t="n">
+        <v>187.6</v>
+      </c>
+      <c r="LB82" s="2" t="n">
+        <v>187.6</v>
+      </c>
+      <c r="LC82" t="n">
         <v>187.6</v>
       </c>
     </row>
@@ -78718,7 +79210,13 @@
       <c r="KZ83" s="2" t="n">
         <v>87.8</v>
       </c>
-      <c r="LA83" t="n">
+      <c r="LA83" s="2" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="LB83" s="2" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="LC83" t="n">
         <v>86.3</v>
       </c>
     </row>
@@ -79661,7 +80159,13 @@
       <c r="KZ84" s="2" t="n">
         <v>25.66</v>
       </c>
-      <c r="LA84" t="n">
+      <c r="LA84" s="2" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="LB84" s="2" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="LC84" t="n">
         <v>25.8</v>
       </c>
     </row>
@@ -80604,7 +81108,13 @@
       <c r="KZ85" s="2" t="n">
         <v>116.6</v>
       </c>
-      <c r="LA85" t="n">
+      <c r="LA85" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="LB85" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="LC85" t="n">
         <v>116</v>
       </c>
     </row>
@@ -81547,7 +82057,13 @@
       <c r="KZ86" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="LA86" t="n">
+      <c r="LA86" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LB86" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LC86" t="n">
         <v>5</v>
       </c>
     </row>
@@ -82490,7 +83006,13 @@
       <c r="KZ87" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="LA87" t="n">
+      <c r="LA87" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LB87" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LC87" t="n">
         <v>7</v>
       </c>
     </row>
@@ -83433,7 +83955,13 @@
       <c r="KZ88" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="LA88" t="n">
+      <c r="LA88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LB88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LC88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -84376,7 +84904,13 @@
       <c r="KZ89" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="LA89" t="n">
+      <c r="LA89" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LB89" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LC89" t="n">
         <v>6</v>
       </c>
     </row>
@@ -85319,7 +85853,13 @@
       <c r="KZ90" s="2" t="n">
         <v>117</v>
       </c>
-      <c r="LA90" t="n">
+      <c r="LA90" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="LB90" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="LC90" t="n">
         <v>110</v>
       </c>
     </row>
@@ -86262,7 +86802,13 @@
       <c r="KZ91" s="2" t="n">
         <v>177</v>
       </c>
-      <c r="LA91" t="n">
+      <c r="LA91" s="2" t="n">
+        <v>189</v>
+      </c>
+      <c r="LB91" s="2" t="n">
+        <v>189</v>
+      </c>
+      <c r="LC91" t="n">
         <v>189</v>
       </c>
     </row>
@@ -87205,7 +87751,13 @@
       <c r="KZ92" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="LA92" t="n">
+      <c r="LA92" s="2" t="n">
+        <v>232</v>
+      </c>
+      <c r="LB92" s="2" t="n">
+        <v>232</v>
+      </c>
+      <c r="LC92" t="n">
         <v>232</v>
       </c>
     </row>
@@ -88148,7 +88700,13 @@
       <c r="KZ93" s="2" t="n">
         <v>67.59999999999999</v>
       </c>
-      <c r="LA93" t="n">
+      <c r="LA93" s="2" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="LB93" s="2" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="LC93" t="n">
         <v>76.3</v>
       </c>
     </row>
@@ -89091,7 +89649,13 @@
       <c r="KZ94" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="LA94" t="n">
+      <c r="LA94" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LB94" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LC94" t="n">
         <v>54</v>
       </c>
     </row>
@@ -90034,7 +90598,13 @@
       <c r="KZ95" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="LA95" t="n">
+      <c r="LA95" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LB95" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LC95" t="n">
         <v>5</v>
       </c>
     </row>
@@ -90977,7 +91547,13 @@
       <c r="KZ96" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="LA96" t="n">
+      <c r="LA96" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LB96" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LC96" t="n">
         <v>4</v>
       </c>
     </row>
@@ -91920,7 +92496,13 @@
       <c r="KZ97" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="LA97" t="n">
+      <c r="LA97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="LB97" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="LC97" t="n">
         <v>37</v>
       </c>
     </row>
@@ -92863,7 +93445,13 @@
       <c r="KZ98" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="LA98" t="n">
+      <c r="LA98" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LB98" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LC98" t="n">
         <v>45</v>
       </c>
     </row>
@@ -93806,7 +94394,13 @@
       <c r="KZ99" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="LA99" t="n">
+      <c r="LA99" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="LB99" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="LC99" t="n">
         <v>49</v>
       </c>
     </row>
@@ -94749,7 +95343,13 @@
       <c r="KZ100" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="LA100" t="n">
+      <c r="LA100" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LB100" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LC100" t="n">
         <v>14</v>
       </c>
     </row>
@@ -95692,7 +96292,13 @@
       <c r="KZ101" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LA101" t="n">
+      <c r="LA101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LB101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LC101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -96635,7 +97241,13 @@
       <c r="KZ102" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="LA102" t="n">
+      <c r="LA102" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="LB102" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="LC102" t="n">
         <v>62.5</v>
       </c>
     </row>

</xml_diff>